<commit_message>
cleaning up files for clustering analysis
</commit_message>
<xml_diff>
--- a/Pipeline_ConceptTrace.xlsx
+++ b/Pipeline_ConceptTrace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeccawilder/Downloads/jatos_mac_java/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A77B7F0-B7DC-D949-A01B-608E229C85BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2727F1-2059-DE44-B8AC-F8F9D40DDAB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13600" yWindow="500" windowWidth="14400" windowHeight="16640" xr2:uid="{ED8E5305-7CF2-E044-9423-C665C0702F10}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>R script</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cleans delayed condition and makes changes to the immediate col identifier </t>
   </si>
   <si>
     <t>cleandata_current.R</t>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t xml:space="preserve">Goes through and removes perseverative errors.  Sets value for perseverative column and excludes row-wise cases.  Ordinal positions </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Writes new file without errors but keeps combined fluency.  Moves combinedflunecy.csv**   </t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F817302E-682A-A842-A053-A46A7028A2AC}">
   <dimension ref="A1:BA94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="T2" sqref="H1:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,134 +502,54 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
       <c r="AV1" s="2"/>
       <c r="AW1" s="2"/>
       <c r="AX1" s="2"/>
@@ -645,137 +565,57 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AN2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AP2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AQ2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
       <c r="AV2" s="2"/>
       <c r="AW2" s="2"/>
       <c r="AX2" s="2"/>
@@ -791,16 +631,16 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -851,22 +691,22 @@
     </row>
     <row r="4" spans="1:53" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -917,15 +757,17 @@
     </row>
     <row r="5" spans="1:53" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>

</xml_diff>